<commit_message>
Laptop 11-June-2018 Registration Page Completed
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/NewToursTestData.xlsx
+++ b/src/main/java/com/qa/testdata/NewToursTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="8460"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="8460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="RegistrationPage" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -27,22 +27,73 @@
     <t>tutorial</t>
   </si>
   <si>
-    <t>TUTORIAL</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test555</t>
-  </si>
-  <si>
-    <t>naveen</t>
-  </si>
-  <si>
-    <t>naveen@123</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>rajesh</t>
+  </si>
+  <si>
+    <t>dahsj</t>
+  </si>
+  <si>
+    <t>dshai</t>
+  </si>
+  <si>
+    <t>warangal</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>rajurajesh</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>uname</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>aa@sdajs.com</t>
+  </si>
+  <si>
+    <t>ads</t>
   </si>
 </sst>
 </file>
@@ -58,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,8 +122,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,13 +137,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -409,78 +482,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -488,12 +489,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Laptop 12-06-2018 Reg Page Update
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/NewToursTestData.xlsx
+++ b/src/main/java/com/qa/testdata/NewToursTestData.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
     <sheet name="RegistrationPage" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="FlightBooking" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -51,9 +51,6 @@
     <t>AP</t>
   </si>
   <si>
-    <t>INDIA</t>
-  </si>
-  <si>
     <t>rajurajesh</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
   </si>
   <si>
     <t>PostalCode</t>
-  </si>
-  <si>
-    <t>Country</t>
   </si>
   <si>
     <t>uname</t>
@@ -124,32 +118,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -159,7 +138,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,9 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -489,10 +466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,54 +482,52 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="M1"/>
+      <c r="N1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -563,7 +538,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -578,19 +553,16 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -600,12 +572,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laptop  13-06-2018:: 00:30-AM Reg Page DDT Done Successfully
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/NewToursTestData.xlsx
+++ b/src/main/java/com/qa/testdata/NewToursTestData.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\Latest Workspace\NewtoursProject\src\main\java\com\qa\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="RegistrationPageData" sheetId="2" r:id="rId2"/>
+    <sheet name="RegistrationData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -112,13 +107,28 @@
   </si>
   <si>
     <t>abc@123</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALBANIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANGOLA </t>
+  </si>
+  <si>
+    <t>aaaaaaaaa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +143,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,10 +178,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -227,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -279,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -473,27 +490,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -515,14 +532,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -531,12 +548,13 @@
     <col min="7" max="7" width="7.5703125" customWidth="1"/>
     <col min="8" max="8" width="8.140625" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -565,16 +583,19 @@
         <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -603,16 +624,19 @@
         <v>505612</v>
       </c>
       <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -640,24 +664,113 @@
       <c r="I3">
         <v>14564561</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>48654654654</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>14564561</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>7445645</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>505612</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="L3" r:id="rId3"/>
-    <hyperlink ref="K3" r:id="rId4"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="M3" r:id="rId3"/>
+    <hyperlink ref="L3" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId5"/>
+    <hyperlink ref="K4" r:id="rId6"/>
+    <hyperlink ref="M4" r:id="rId7"/>
+    <hyperlink ref="L4" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Home Page Basic Done
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/NewToursTestData.xlsx
+++ b/src/main/java/com/qa/testdata/NewToursTestData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
     <sheet name="RegistrationData" sheetId="2" r:id="rId2"/>
+    <sheet name="FlightBookingData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>username</t>
   </si>
@@ -122,13 +123,76 @@
   </si>
   <si>
     <t>aaaaaaaaa</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>fromMonth</t>
+  </si>
+  <si>
+    <t>fromDay</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>toMonth</t>
+  </si>
+  <si>
+    <t>toDay</t>
+  </si>
+  <si>
+    <t>Airlines</t>
+  </si>
+  <si>
+    <t>Passengers</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>No Preference</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Unified Airlines</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Pangea Airlines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +214,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,11 +256,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +581,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,10 +591,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -535,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,43 +635,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -602,7 +682,7 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>7445645</v>
       </c>
       <c r="D2" t="s">
@@ -620,7 +700,7 @@
       <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>505612</v>
       </c>
       <c r="J2" t="s">
@@ -646,7 +726,7 @@
       <c r="C3">
         <v>48654654654</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
@@ -664,16 +744,16 @@
       <c r="I3">
         <v>14564561</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -687,7 +767,7 @@
       <c r="C4">
         <v>48654654654</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E4" t="s">
@@ -705,16 +785,16 @@
       <c r="I4">
         <v>14564561</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -746,7 +826,7 @@
       <c r="I5">
         <v>505612</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K5" t="s">
@@ -773,4 +853,134 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="5">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="5">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="5">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>